<commit_message>
- USER LOGIN AND LOGOUT ROUTE WORKED OUT - GENRE PAGE FIXED - ADDED WORKING LINKS
</commit_message>
<xml_diff>
--- a/public/resources/Strategy.xlsx
+++ b/public/resources/Strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psn\Desktop\Web Development\Game-hub-server\public\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF1A1D0-4D44-460E-A481-DE16823E3E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDEE546-7F1A-4941-9D81-D2B60E0DFEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" activeTab="2" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
   <si>
     <t>NAME</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Dynasty War is the conflict of Three Kingdoms in the ravaged land of Han Dynasty. Choose one out of the four rulers to take initiative and conquer the entire map.</t>
   </si>
   <si>
-    <t>Fight your rivals in increasingly difficult battles, using 3 from 8 officers you can cycle, 8 warrior types, buildings, sorceries, other upgrades, and control your army’s movement using two different modes for advanced tactics. Rewrite history and be the Emperor of the Chinese land!</t>
-  </si>
-  <si>
     <t>ABOUT</t>
   </si>
   <si>
@@ -282,6 +279,48 @@
   </si>
   <si>
     <t>Age of Tanks Warriors: TD War is an epic tower defense game where tanks reign supreme, crafting their own civilization across parallel universes. Evolve your tanks through ages, from Stone Age warriors to modern marvels. Dominate the battlefield with strategic prowess, upgrading your army and conquering enemies in epic 1v1 battles. Unleash your inner tactician and lead your tanks to victory in this strategic saga.</t>
+  </si>
+  <si>
+    <t>"images/endlessseige.jpg"</t>
+  </si>
+  <si>
+    <t>"images\\millionarequiz.jpg"</t>
+  </si>
+  <si>
+    <t>"images\\13nights.jpg"</t>
+  </si>
+  <si>
+    <t>"images\\stickmanarmy.jpg"</t>
+  </si>
+  <si>
+    <t>"images\\imposterwars.jpg"</t>
+  </si>
+  <si>
+    <t>"images\\airtraffic.jpg"</t>
+  </si>
+  <si>
+    <t>"images\\warlands.jpg"</t>
+  </si>
+  <si>
+    <t>"images//plants.jpg"</t>
+  </si>
+  <si>
+    <t>"images//dynastywar.jpg"</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/mahjong_dynasty_html5</t>
+  </si>
+  <si>
+    <t>"images//mahjongdynasty.jpg"</t>
+  </si>
+  <si>
+    <t>Mahjong Dynasty</t>
+  </si>
+  <si>
+    <t>MAHJONG DYNASTY, a journey through Asia. Connect Mahjong tiles to clear the board. Make mah jong connections and complete all levels with 3 stars.</t>
+  </si>
+  <si>
+    <t>"images\\draughts.jpg"</t>
   </si>
 </sst>
 </file>
@@ -366,14 +405,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -707,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D1A3C6-19CA-40FA-BFCB-1422A2C32063}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -738,7 +774,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="100.3" x14ac:dyDescent="0.4">
@@ -752,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
@@ -766,7 +802,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
@@ -780,7 +816,7 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="162" x14ac:dyDescent="0.4">
@@ -794,7 +830,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="154.30000000000001" x14ac:dyDescent="0.4">
@@ -808,7 +844,7 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="285.45" x14ac:dyDescent="0.4">
@@ -822,7 +858,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="169.75" x14ac:dyDescent="0.4">
@@ -836,7 +872,7 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
@@ -850,12 +886,21 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
-      <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -882,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -890,13 +935,13 @@
     </row>
     <row r="2" spans="1:4" ht="100.3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -904,13 +949,13 @@
     </row>
     <row r="3" spans="1:4" ht="162" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -918,13 +963,13 @@
     </row>
     <row r="4" spans="1:4" ht="378" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -932,13 +977,13 @@
     </row>
     <row r="5" spans="1:4" ht="46.3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -946,13 +991,13 @@
     </row>
     <row r="6" spans="1:4" ht="108" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -960,43 +1005,43 @@
     </row>
     <row r="7" spans="1:4" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C11" s="4"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C12" s="4"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1007,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA54E530-E41A-4D11-80A2-CF2E736F99BE}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1028,102 +1073,105 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="274.3" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="342.9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="8" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>73</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
         <v>77</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
         <v>80</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixed driving_index page - fixed minor bugs - requires styling
</commit_message>
<xml_diff>
--- a/public/resources/Strategy.xlsx
+++ b/public/resources/Strategy.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psn\Desktop\Web Development\Game-hub-server\public\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDEE546-7F1A-4941-9D81-D2B60E0DFEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7FCD75-D581-4A8C-BCC7-5026E812A57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" activeTab="6" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
     <sheet name="Puzzle" sheetId="2" r:id="rId2"/>
     <sheet name="Action" sheetId="3" r:id="rId3"/>
+    <sheet name="Driving" sheetId="4" r:id="rId4"/>
+    <sheet name="Fighting" sheetId="5" r:id="rId5"/>
+    <sheet name="Shooting" sheetId="6" r:id="rId6"/>
+    <sheet name="Sports" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="268">
   <si>
     <t>NAME</t>
   </si>
@@ -321,6 +325,525 @@
   </si>
   <si>
     <t>"images\\draughts.jpg"</t>
+  </si>
+  <si>
+    <t>Retro Garage — Car Mechanic</t>
+  </si>
+  <si>
+    <t>Retro Garage – Car Mechanic is an engaging simulation game that lets players step into the shoes of a professional car mechanic. The game offers a detailed and immersive experience, offering a wide range of classic cars to repair, restore and customize. Players can diagnose mechanical issues, order replacement parts, and perform hands-on repairs and upgrades. With its clear graphics and comprehensive yet easy-to-understand gameplay mechanics, Retro Garage – Car Mechanic appeals to both automotive enthusiasts and casual gamers looking for a challenging yet rewarding virtual workshop environment.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/retro_garage_car_mechanic</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/supra_drift_3d</t>
+  </si>
+  <si>
+    <t>Supra Drift 3D</t>
+  </si>
+  <si>
+    <t>Supra Drift 3D is a great opportunity to take spin in the famous Toyota Supra. In this game you won't only have the freedom to drive around, but also bring a personal touch to it. You can first pick a color, choose a cool body-kit and then go tune it! This beast of a machine is good for both racing and drifting. With a realistic city environment waiting for you, you'll get the chance to burn some rubber anywhere you want. No annoying traffic or chance that you run out of fuel. Just have fun!</t>
+  </si>
+  <si>
+    <t>City Rider</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/city_rider</t>
+  </si>
+  <si>
+    <t>City Rider is a fun driving game on busy and empty streets too. Drive in different cities with 9 different cars. You have race cars, buses, trucks, and more! You will also have the choice of 3 different maps, each one with unique features.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/traffic_jam_3d</t>
+  </si>
+  <si>
+    <t>Traffic Jam 3D</t>
+  </si>
+  <si>
+    <t>Traffic Jam 3D is a realistic driving game in which you must navigate a busy highway. Your goal is to reach your destination at a given time. You'll earn money for all the successful races that you've done. With the money that you will earn, you can upgrade your current car, or you can even purchase a new ride with better performance and specifications. Don't forget to buy nitro to give yourself an advantage!</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/racing_car_driving_car</t>
+  </si>
+  <si>
+    <t>Racing Car Driving Car</t>
+  </si>
+  <si>
+    <t>Savor the Simulator of New Racing Car Games. A wide variety of racing vehicles, including police cars and GT cars, are driven quickly on city roadways. Take a look at the racing car simulator in digital games. Play around the city's roads and take pleasure in driving fast cars in enjoyable racing games. You can have the unique experience of driving real sports cars on one of the many unique asphalt tracks by using the Drive Racing Sport Evolution Simulator.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/gangster_hero</t>
+  </si>
+  <si>
+    <t>Gangster Hero is a super open-world game where you are going to explore a massive, immersive, and gangster city. You have to survive against the city mafia. You can buy new vehicles and drive different motorcycles and cars. Play this 3D game at Y8 now and have fun.</t>
+  </si>
+  <si>
+    <t>Gangster Hero</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/city_stunts</t>
+  </si>
+  <si>
+    <t>City Stunts</t>
+  </si>
+  <si>
+    <t>Careen through the town center in City Stunts and look for the best ramps and super loops to try. Speed through the loops and try not to lose traction, or race up the ramps and jump high enough to leap straight over the rooftops. You can see the various vert ramps and loops poking out from among the houses, so if you spot one that looks good you can set out find it by taking the right turns through the streets and alleys. Make sure you have a good run-up and perform the most amazing stunts in this thrilling 3D car game!</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/night_city_racing</t>
+  </si>
+  <si>
+    <t>Night City Racing</t>
+  </si>
+  <si>
+    <t>Now is your chance to drive super realistic car driving simulation with Night City Racing game! Drive a total of 10 extremely fast sports car which you can play in a racing mode, challenge mode or simply free ride. Get in the garage and customize every detail, the color, the engine or the bodyworks. Step on the gas and race to the full adrenaline on the race track! Win the race and upgrade cars! </t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/grand_theft_blockworld</t>
+  </si>
+  <si>
+    <t>Grand Theft Blockworld</t>
+  </si>
+  <si>
+    <t>Grand Theft Blockworld - Amazing 3D game with a fast car and many obstacles on a track. Drive carefully to avoid obstacles and difficult places on the track. Each level has time, you must reach the finish line before the time runs out. Join now and complete all the interesting game levels. </t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/revolution_offroad</t>
+  </si>
+  <si>
+    <t>Revolution Offroad</t>
+  </si>
+  <si>
+    <t>Revolution Offroad is a car simulator adventure game! Your goal is to safely navigate your off-road truck to the finish line without crashing. Keep an eye on your gas tank, and earn rewards for each completed level. With career, time attack and free mode options, use your rewards to upgrade your current vehicle or purchase new ones. Navigate the rugged terrain with skill and precision as you take your off-road ride to the next level.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/city_car_stunt_3</t>
+  </si>
+  <si>
+    <t>City Car Stunt 3</t>
+  </si>
+  <si>
+    <t>City Car Stunt continues with the 3rd game with improved physics. Also, City Car Stunt 3 is more enjoyable with more realistic and dazzling cars! Try to complete 6 different routes in the game before time runs out! Each level unlocks a new car and make you more powerful for upcoming levels! You have to race against time to win the fastest car!</t>
+  </si>
+  <si>
+    <t>Show off your skills in the newly designed huge "Free Driving" map. On this map, you can play games like darts, soccer and bowling with your car. You can just perform a few cool stunts without being pressed for time in the free driving mode. Use the ramps to fly your car!</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/apex_football_battle</t>
+  </si>
+  <si>
+    <t>Apex Football Battle</t>
+  </si>
+  <si>
+    <t>Play the most realistic and complete football simulation experience ever made, the Apex Football Battle, where the excitement of the beautiful game comes to life. Experience the thrill of pure, unadulterated football action by delving into the world of friendly matches.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/penalty_kicks</t>
+  </si>
+  <si>
+    <t>Penalty Kicks</t>
+  </si>
+  <si>
+    <t>Hey you soccer fans out there! Want to practice your kicks? Well Penalty Kicks is the game for you. This game can be played on both computer and mobile so you can practice anytime you like. See if you can goal more than the others in the leaderboard!</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/football_legends_2016</t>
+  </si>
+  <si>
+    <t>Football Legends 2016</t>
+  </si>
+  <si>
+    <t>Make a goal and win the tournament.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/cricket_superstar_league</t>
+  </si>
+  <si>
+    <t>Cricket Superstar League</t>
+  </si>
+  <si>
+    <t>Hello cricket fans, Cricket Superstar League is the game for you! This is a fun 3D cricket game that you can have the real life feel on playing the sport. Select between levels Infinite Challenges and Full Match. From Infinite Challenges you can choose between Easy, Medium and Hard Mode. While in full match, choose the opponent team you wish to defeat. Pick your favorite team and win all the matches. Play now!</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/let_s_play_soccer</t>
+  </si>
+  <si>
+    <t>Let's Play Soccer</t>
+  </si>
+  <si>
+    <t>Come and try "Cool Goal"-a football game that tests your aiming, shooting, and layout logic! Your task is to ensure that the ball is delivered to the goal accurately every time. To do this, you need to avoid the enemy's defense countless times, and they will do everything possible to stand between you and the goal post! Experience a brand new "football game" while testing your brainpower and football skills.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/azad_cricket</t>
+  </si>
+  <si>
+    <t>Azad Cricket</t>
+  </si>
+  <si>
+    <t>Azad Cricket - Welcome to fun sports game, championship about one player and you will have to score maximum boundaries to win the cricket championship. Control your mouse to hit the ball, but control the force of the throw so as not to fly out.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/football_legends_2019</t>
+  </si>
+  <si>
+    <t>Football Legends 2019</t>
+  </si>
+  <si>
+    <t>Since you loved the first Football Legends, we give you this 2019 update! With new players in each team. You'll definitely love this new addition in the Football Legends series. Complete all the achievements, finish the tournament as the champion or you can play in random. Play against your friends 1 vs 1, 2 vs 2 or 1 vs 2! Get the highest score and be in the leaderboard.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/soccer_skills_euro_cup_2021_edition</t>
+  </si>
+  <si>
+    <t>Soccer Skills: Euro Cup 2021 Edition</t>
+  </si>
+  <si>
+    <t>Play the best soccer tournament game in Soccer Skills: Euro Cup 2021 Edition. Select your favorite country, prepare your team hard and win game after game as you go through the round until you reach the grand final of the championship. Move your players around the field while still pressing on them and when you have the ball pass it to a teammate or shoot directly at the goal to score a goal. Make use of all your soccer skills and take to the field to win all the matches.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/cpl_tournament_2020</t>
+  </si>
+  <si>
+    <t>CPL Tournament 2020</t>
+  </si>
+  <si>
+    <t>CPL tournament 2020 is for cricket lovers and its back with a new challenge. Grab your bat and ball its time to play cricket premier league tournament. Choose to play Single match or the Cup Series. Just choose your IPL (Indian premier league) team and get started. You can play 2, 5 or 10 overs. Just tap on the screen to take a shot. You have to win 4 matches to reach the quarterfinal. In every match, you have to chase a target of specific balls. With great graphics and awesome sounds effects, you gonna love this cricket game. So start hitting big sixes with CPL Tournament 2020 and enjoy playing this game</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/sniper_vs_sniper</t>
+  </si>
+  <si>
+    <t>Sniper vs Sniper</t>
+  </si>
+  <si>
+    <t>Sniper vs Sniper is a sniper shooter game where you need to show your sniper shooting skills to defeat your enemy. Choose a sniper gun or buy a new one in the game shop. Aim well to hit the opponent and avoid obstacles. </t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/_a_rifleman_from_ireland</t>
+  </si>
+  <si>
+    <t>A Rifleman From Ireland</t>
+  </si>
+  <si>
+    <t>The game revolves around the heroic journey of an Irish man, dedicated to defending his beloved country against a relentless invasion by enemies. Play as the courageous character and navigate through tricky terrains and prepare to engage in a shooting spree against enemy forces. Uncover the motives behind the invasion and witness the determination of our hero as he fights to preserve his nation’s freedom. Get ready to experience the thrill of battle and showcase your skills as a true hero. </t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/funny_shooter_3d</t>
+  </si>
+  <si>
+    <t>Funny Shooter 3D</t>
+  </si>
+  <si>
+    <t>Funny Shooter 3D is a fun 3d FPS shooter game! Get your guns ready and survive the attack of the red army. Use different guns in your arsenal to defend yourself from heavy attacks. Eliminate all the enemies to advance to the next level. </t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/skibidi_toilet_bullet</t>
+  </si>
+  <si>
+    <t>Skibidi Toilet Bullet</t>
+  </si>
+  <si>
+    <t>Skibidi Toilet Bullet is an exhilarating and addictive mobile game that plunges players into a world of precision aiming, strategic thinking, and physics-based challenges. Set in a stylish and cartoonish environment, the game combines puzzle-solving and action gameplay elements to create a unique and engaging experience.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/apple_shooter</t>
+  </si>
+  <si>
+    <t>Apple Shooter</t>
+  </si>
+  <si>
+    <t>Apple Shooter is an HTML5 archery game that will test your skills as an Indian warrior. Being a sharp-shooter is what this game needs since the life of your friend depends on how well you target the apple. Every time you hit the apple, the distance between you and your friend will be farther. Also, there will be some sort of a barricade to make the difficulty more advanced. Your friend's life is at risk. There's no room for mistakes so be brave and be sharp enough to target the apple and try not to kill your dear friend. Take your time in controlling the power and direction of the bow to perfect the shot and save your friend. You can play this exciting game on your mobile phones such as iPhone, Android, and even on your iPads, cool right? Play this addicting game and become an amazing Indian warrior!</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/command_strike_fps</t>
+  </si>
+  <si>
+    <t>Command Strike Fps</t>
+  </si>
+  <si>
+    <t>Command Strike Fps is an intense army shooting FPS game. Enjoy the fun features in this game, and become a commando in this mission! Here you’ll find classic and favorite features of shooting games. About Command Strike FPS, Explore various maps, games modes. Gear up your powerful guns Destroy your enemies and conquer the area. Aim and strike the enemies and do not let them kill you.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/masked_forces_unlimited</t>
+  </si>
+  <si>
+    <t>Masked Forces Unlimited</t>
+  </si>
+  <si>
+    <t>A new generation of FPS game which you can play as campaign or multiplayer against online users. Gear up your avatar and win the different modes by earning a highest score.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/polyblicy</t>
+  </si>
+  <si>
+    <t>Polyblicy</t>
+  </si>
+  <si>
+    <t>Polyblicy is an amazing first-person shooter game with many different guns and heroes. Play this funny shooter game with your friends and try to become a champion among online players. Throw grenades and switch between different weapons.</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/roblox_world_shooter</t>
+  </si>
+  <si>
+    <t>Roblox World Shooter</t>
+  </si>
+  <si>
+    <t>Manage your little character and see him through the never-ending conflict in Mini Obby War Game, an action-packed 3D game set in a Roblox environment. With over ten unique and challenging levels, this amazing game is within your reach. Keep sprinting to avoid being caught by the waves of enemy troops who will shoot you if they see you, and aim and fire at all adversaries. As you defeat enemies, youll find coins that may be used to unlock additional characters with unique abilities. </t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/call_of_ops_2</t>
+  </si>
+  <si>
+    <t>Call of Ops 2 features next-gen graphics, lots of highly detailed maps, and a big arsenal of powerful weapons to shoot rival players in deathmatch game mode. As you fight, you earn money and you can use this money to purchase upgrades and new weapons. Try to rack up as many kills as possible and dominate the arena against other players from around the world.</t>
+  </si>
+  <si>
+    <t>Call of Ops 2</t>
+  </si>
+  <si>
+    <t>https://agamecdn.com/system/static/thumbs/spil_thumb_big/33774/thumb_92_200X120_173444_1569397450.jpg?1692361591</t>
+  </si>
+  <si>
+    <t>https://agamecdn.com/system/static/thumbs/spil_thumb_big/90455/webp_Madness-Driver-Vertigo-City-200x120.webp?1713267005</t>
+  </si>
+  <si>
+    <t>https://images.crazygames.com/shadow-ninja-revenge/20230501110202/shadow-ninja-revenge-cover?auto=format%2Ccompress&amp;q=90&amp;cs=strip&amp;ch=DPR&amp;w=178&amp;h=100&amp;fit=crop</t>
+  </si>
+  <si>
+    <t>https://agamecdn.com/system/static/thumbs/spil_thumb_big/90658/jpeg_Hydro-Racing-3D-200x120.jpg?1714992970</t>
+  </si>
+  <si>
+    <t>https://agamecdn.com/system/static/thumbs/spil_thumb_big/31860/jpeg_200X120_167965.jpg?1692360335</t>
+  </si>
+  <si>
+    <t>https://agamecdn.com/system/static/thumbs/spil_thumb_big/71853/thumb_92_Dirt-Bike-Racing-Duel-200x120.jpg?1692362970</t>
+  </si>
+  <si>
+    <t>https://images.crazygames.com/games/10-minutes-till-dawn/cover-1652811077990.png?auto=format%2Ccompress&amp;q=90&amp;cs=strip&amp;ch=DPR&amp;w=178&amp;h=100&amp;fit=crop</t>
+  </si>
+  <si>
+    <t>https://images.crazygames.com/age-of-tanks-warriors-td-war_16x9/20240424032706/age-of-tanks-warriors-td-war_16x9-cover?auto=format%2Ccompress&amp;q=90&amp;cs=strip&amp;ch=DPR&amp;w=178&amp;h=100&amp;fit=crop</t>
+  </si>
+  <si>
+    <t>KOF Fighting</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/kof_fighting</t>
+  </si>
+  <si>
+    <t>To become the king of fighter, one have to survive many fightings. Every fighting will make him more powerful! Would you like to have a try?</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/28384/small.jpg</t>
+  </si>
+  <si>
+    <t>Squid Game Multiplayer Fighting</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/squid_game_multiplayer_fighting</t>
+  </si>
+  <si>
+    <t>Squid Game Multiplayer Fighting - Epic street battle with Squid players. You can join and play with your friend together. Choose your character and buy new items to customize your game. Select the game mode and play this squid game on Y8 with fun. Collect oranges to buy new skins for your character.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/146233/small.gif</t>
+  </si>
+  <si>
+    <t>Ultimate Fighting</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/ultimate_fighting</t>
+  </si>
+  <si>
+    <t>The new fighting game has new moves, even strokes and more enjoyable. There are a variety of roles and different occupations for you to choose, like soldiers, gunmen, warrior, mage, assassin. At the same time, and the game also supports double mode, So let you and your partner to play together. Carry on a PK contest to see who is the strongest when you and your little friends play tired. Very challenging game, Call on your little partner join it and fighting together.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/56860/small.gif</t>
+  </si>
+  <si>
+    <t>Stickman Fighting</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/stickman_fighting</t>
+  </si>
+  <si>
+    <t>In the world of stickman, everyone must take the severe fighting test in their 18-year-old coming-of-age ceremony. Only those brave ones who can go through the severe test can be a real stickman hero. Let's follow the stickman fighting test now!</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/58159/small.gif</t>
+  </si>
+  <si>
+    <t>Mutant Fighting Arena</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/mutant_fighting_arena</t>
+  </si>
+  <si>
+    <t>Earn crystals by winning enough matches and then spend them to unlock new mutants with unique attacks and abilities. Level up your mutants by fighting battles, and spend coins to unlock new skills and make them stronger than ever before.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/103184/small.gif</t>
+  </si>
+  <si>
+    <t>Comic Stars Fighting 3</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/comic_stars_fighting_3</t>
+  </si>
+  <si>
+    <t>Comic Stars Fighting 3 is an excellent fighting game in which you can choose both single mode fighting and 2 players fighting. Come to choose your favorite character and fight with your friends! Experience the excitement of being a knight, killing enemies using your stunning magic Kung Fu skills. Let's see who can survive at last!</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/54134/small.gif</t>
+  </si>
+  <si>
+    <t>Ninjago Legend Fighting 2</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/ninjago_legend_fighting_2</t>
+  </si>
+  <si>
+    <t>This is Ninjago game. Kai lost in mysterious forests, where many enemies are waiting, Kai's mission is to fight against his enemies with special abilities. Help Kai finish all levels in game.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/55512/small.gif</t>
+  </si>
+  <si>
+    <t>Creetor Animation Fighting</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/creetor_animation_fighting_luffy_vs_naruto</t>
+  </si>
+  <si>
+    <t>Best animation fighting game ever! You can choose your character from One piece,naruto,bleach,dragon ball characters to fight computer or your friends.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/66660/small.gif</t>
+  </si>
+  <si>
+    <t>Dead Samurai</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/dead_samurai</t>
+  </si>
+  <si>
+    <t>Samurai sword duel fighting. Battle nine samurai with eight stances and over 40 attacks. Three bonus rounds. Inspired by classic arcade 2D fighting games.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/88313/small.gif</t>
+  </si>
+  <si>
+    <t>Gang Fall Party</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/gang_fall_party</t>
+  </si>
+  <si>
+    <t>Gang Fall Party - Welcome to very fun io fighting game with many opponents. Punch your opponents to get stronger as you take down each opponent. Fight against all opponents or play with your friend. Become the best fighter in this 3D gang game. Play with fun.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143824/small.gif</t>
+  </si>
+  <si>
+    <t>Chroma Wars</t>
+  </si>
+  <si>
+    <t>https://www.y8.com/games/chroma_wars</t>
+  </si>
+  <si>
+    <t>Place your units to best protect yourself as a whole. Attack and take control of enemy bases.</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/6796/small.jpg</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/152012/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/173717/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/126458/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169035/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/156863/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/170213/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/116213/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/151868/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/150314/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/160971/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/133765/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/140066/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/175019/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/170907/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/111441/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/153528/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/114977/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/166799/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/141997/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/164491/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/173303/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169177/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs-small-thumbnails-001/107080/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/y8-thumbs/71600/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/127780/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/138142/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/145697/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/121122/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/141954/small.gif</t>
+  </si>
+  <si>
+    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143474/small.gif</t>
   </si>
 </sst>
 </file>
@@ -405,7 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -426,6 +949,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -743,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D1A3C6-19CA-40FA-BFCB-1422A2C32063}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1052,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA54E530-E41A-4D11-80A2-CF2E736F99BE}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1076,11 +1606,14 @@
       <c r="A2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="342.9" x14ac:dyDescent="0.4">
@@ -1107,6 +1640,9 @@
       <c r="C4" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="D4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -1118,6 +1654,9 @@
       <c r="C5" t="s">
         <v>64</v>
       </c>
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
@@ -1129,6 +1668,9 @@
       <c r="C6" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
@@ -1140,6 +1682,9 @@
       <c r="C7" s="7" t="s">
         <v>71</v>
       </c>
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
@@ -1151,6 +1696,9 @@
       <c r="C8" t="s">
         <v>73</v>
       </c>
+      <c r="D8" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
@@ -1162,6 +1710,9 @@
       <c r="C9" t="s">
         <v>77</v>
       </c>
+      <c r="D9" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
@@ -1172,6 +1723,708 @@
       </c>
       <c r="C10" t="s">
         <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D6D956F9-E049-4AF2-BF91-ABF570747F3A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3A6348-4879-4FC1-9CC7-025FE79B3684}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="347.15" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="108" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="239.15" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="192.9" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="154.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="223.75" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="169.75" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
+      <c r="C13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DFBDDC-6B65-4A2E-9ED5-E421D7822BA2}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C70367C-4436-465B-8856-B0A5BA258AAC}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="115.75" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="270" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="177.45" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="401.15" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="246.9" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30E7259-0B3B-43AD-AD0A-966BC176F937}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="23.15" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="216" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="185.15" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="239.15" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="308.60000000000002" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- all pending changes done - added search feature - fixed home page - only need to add urls to home page games
</commit_message>
<xml_diff>
--- a/public/resources/Strategy.xlsx
+++ b/public/resources/Strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psn\Desktop\Web Development\Game-hub-server\public\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7FCD75-D581-4A8C-BCC7-5026E812A57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121915AD-0FB4-437B-B194-24D7C54180CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" activeTab="6" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" activeTab="7" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Fighting" sheetId="5" r:id="rId5"/>
     <sheet name="Shooting" sheetId="6" r:id="rId6"/>
     <sheet name="Sports" sheetId="7" r:id="rId7"/>
+    <sheet name="All" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="268">
   <si>
     <t>NAME</t>
   </si>
@@ -633,9 +634,6 @@
     <t>To become the king of fighter, one have to survive many fightings. Every fighting will make him more powerful! Would you like to have a try?</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/28384/small.jpg</t>
-  </si>
-  <si>
     <t>Squid Game Multiplayer Fighting</t>
   </si>
   <si>
@@ -645,9 +643,6 @@
     <t>Squid Game Multiplayer Fighting - Epic street battle with Squid players. You can join and play with your friend together. Choose your character and buy new items to customize your game. Select the game mode and play this squid game on Y8 with fun. Collect oranges to buy new skins for your character.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/146233/small.gif</t>
-  </si>
-  <si>
     <t>Ultimate Fighting</t>
   </si>
   <si>
@@ -657,9 +652,6 @@
     <t>The new fighting game has new moves, even strokes and more enjoyable. There are a variety of roles and different occupations for you to choose, like soldiers, gunmen, warrior, mage, assassin. At the same time, and the game also supports double mode, So let you and your partner to play together. Carry on a PK contest to see who is the strongest when you and your little friends play tired. Very challenging game, Call on your little partner join it and fighting together.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/56860/small.gif</t>
-  </si>
-  <si>
     <t>Stickman Fighting</t>
   </si>
   <si>
@@ -669,9 +661,6 @@
     <t>In the world of stickman, everyone must take the severe fighting test in their 18-year-old coming-of-age ceremony. Only those brave ones who can go through the severe test can be a real stickman hero. Let's follow the stickman fighting test now!</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/58159/small.gif</t>
-  </si>
-  <si>
     <t>Mutant Fighting Arena</t>
   </si>
   <si>
@@ -681,9 +670,6 @@
     <t>Earn crystals by winning enough matches and then spend them to unlock new mutants with unique attacks and abilities. Level up your mutants by fighting battles, and spend coins to unlock new skills and make them stronger than ever before.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/103184/small.gif</t>
-  </si>
-  <si>
     <t>Comic Stars Fighting 3</t>
   </si>
   <si>
@@ -693,9 +679,6 @@
     <t>Comic Stars Fighting 3 is an excellent fighting game in which you can choose both single mode fighting and 2 players fighting. Come to choose your favorite character and fight with your friends! Experience the excitement of being a knight, killing enemies using your stunning magic Kung Fu skills. Let's see who can survive at last!</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/54134/small.gif</t>
-  </si>
-  <si>
     <t>Ninjago Legend Fighting 2</t>
   </si>
   <si>
@@ -705,9 +688,6 @@
     <t>This is Ninjago game. Kai lost in mysterious forests, where many enemies are waiting, Kai's mission is to fight against his enemies with special abilities. Help Kai finish all levels in game.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/55512/small.gif</t>
-  </si>
-  <si>
     <t>Creetor Animation Fighting</t>
   </si>
   <si>
@@ -717,9 +697,6 @@
     <t>Best animation fighting game ever! You can choose your character from One piece,naruto,bleach,dragon ball characters to fight computer or your friends.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/66660/small.gif</t>
-  </si>
-  <si>
     <t>Dead Samurai</t>
   </si>
   <si>
@@ -729,9 +706,6 @@
     <t>Samurai sword duel fighting. Battle nine samurai with eight stances and over 40 attacks. Three bonus rounds. Inspired by classic arcade 2D fighting games.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/88313/small.gif</t>
-  </si>
-  <si>
     <t>Gang Fall Party</t>
   </si>
   <si>
@@ -741,9 +715,6 @@
     <t>Gang Fall Party - Welcome to very fun io fighting game with many opponents. Punch your opponents to get stronger as you take down each opponent. Fight against all opponents or play with your friend. Become the best fighter in this 3D gang game. Play with fun.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143824/small.gif</t>
-  </si>
-  <si>
     <t>Chroma Wars</t>
   </si>
   <si>
@@ -753,97 +724,127 @@
     <t>Place your units to best protect yourself as a whole. Attack and take control of enemy bases.</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/6796/small.jpg</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/152012/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/173717/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/126458/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169035/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/156863/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/170213/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/116213/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/151868/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/150314/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/160971/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/133765/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/140066/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/175019/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/170907/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/111441/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/153528/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/114977/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/166799/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/141997/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/164491/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/173303/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169177/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/y8-thumbs-small-thumbnails-001/107080/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/y8-thumbs/71600/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/127780/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/138142/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/145697/small.gif</t>
-  </si>
-  <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/121122/small.gif</t>
-  </si>
-  <si>
     <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/141954/small.gif</t>
   </si>
   <si>
-    <t>https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143474/small.gif</t>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/173717/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/126458/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169035/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/152012/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/156863/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/170213/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/116213/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/151868/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/150314/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/160971/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/133765/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/28384/small.jpg"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/146233/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/56860/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/58159/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/103184/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/54134/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/55512/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/66660/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/88313/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143824/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/6796/small.jpg"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/173303/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/164491/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/141997/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/166799/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/114977/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/153528/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/111441/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/170907/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/175019/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/140066/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169177/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs-small-thumbnails-001/107080/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/y8-thumbs/71600/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/127780/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/138142/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/145697/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/121122/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143474/small.gif"</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1275,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1444,7 +1445,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1583,7 +1584,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1741,7 +1742,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1771,7 +1772,7 @@
         <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
@@ -1784,8 +1785,8 @@
       <c r="C3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D3" t="s">
-        <v>240</v>
+      <c r="D3" s="12" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="108" x14ac:dyDescent="0.4">
@@ -1798,8 +1799,8 @@
       <c r="C4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D4" t="s">
-        <v>241</v>
+      <c r="D4" s="12" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
@@ -1812,8 +1813,8 @@
       <c r="C5" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D5" t="s">
-        <v>238</v>
+      <c r="D5" s="12" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="239.15" x14ac:dyDescent="0.4">
@@ -1826,8 +1827,8 @@
       <c r="C6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D6" t="s">
-        <v>242</v>
+      <c r="D6" s="12" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
@@ -1841,7 +1842,7 @@
         <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
@@ -1855,7 +1856,7 @@
         <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="192.9" x14ac:dyDescent="0.4">
@@ -1869,7 +1870,7 @@
         <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="154.30000000000001" x14ac:dyDescent="0.4">
@@ -1883,7 +1884,7 @@
         <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="223.75" x14ac:dyDescent="0.4">
@@ -1897,7 +1898,7 @@
         <v>124</v>
       </c>
       <c r="D11" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="169.75" x14ac:dyDescent="0.4">
@@ -1911,7 +1912,7 @@
         <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
@@ -1920,8 +1921,14 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/156863/small.gif" xr:uid="{B38A2F70-B33B-4910-9F0C-880DF095E349}"/>
+    <hyperlink ref="D5" r:id="rId2" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/152012/small.gif" xr:uid="{7D9600C1-96CA-45C4-B64B-D186EDFC42F2}"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169035/small.gif" xr:uid="{48AB55D2-ABA7-4C01-8C91-180B09126D19}"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/126458/small.gif" xr:uid="{799C108D-B504-48B0-82B2-D909874AD226}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1930,7 +1937,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1960,147 +1967,147 @@
         <v>196</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
         <v>198</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>199</v>
       </c>
-      <c r="C3" t="s">
-        <v>200</v>
-      </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
         <v>202</v>
       </c>
-      <c r="B4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" t="s">
-        <v>204</v>
-      </c>
       <c r="D4" t="s">
-        <v>205</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D10" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D12" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2112,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C70367C-4436-465B-8856-B0A5BA258AAC}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2143,7 +2150,7 @@
         <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="270" x14ac:dyDescent="0.4">
@@ -2157,7 +2164,7 @@
         <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
@@ -2171,7 +2178,7 @@
         <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="177.45" x14ac:dyDescent="0.4">
@@ -2185,7 +2192,7 @@
         <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="401.15" x14ac:dyDescent="0.4">
@@ -2213,7 +2220,7 @@
         <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
@@ -2227,7 +2234,7 @@
         <v>176</v>
       </c>
       <c r="D8" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
@@ -2241,7 +2248,7 @@
         <v>179</v>
       </c>
       <c r="D9" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="246.9" x14ac:dyDescent="0.4">
@@ -2255,7 +2262,7 @@
         <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
@@ -2269,7 +2276,7 @@
         <v>184</v>
       </c>
       <c r="D11" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2281,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30E7259-0B3B-43AD-AD0A-966BC176F937}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2312,7 +2319,7 @@
         <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
@@ -2326,7 +2333,7 @@
         <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="23.15" x14ac:dyDescent="0.4">
@@ -2340,7 +2347,7 @@
         <v>137</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="216" x14ac:dyDescent="0.4">
@@ -2354,7 +2361,7 @@
         <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
@@ -2368,7 +2375,7 @@
         <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
@@ -2382,7 +2389,7 @@
         <v>146</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="185.15" x14ac:dyDescent="0.4">
@@ -2396,7 +2403,7 @@
         <v>149</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="239.15" x14ac:dyDescent="0.4">
@@ -2409,8 +2416,8 @@
       <c r="C9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D9" t="s">
-        <v>266</v>
+      <c r="D9" s="12" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="308.60000000000002" x14ac:dyDescent="0.4">
@@ -2428,6 +2435,984 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{83ECC319-8DD8-4974-B87F-769CB8BC6D7A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55908B1F-4066-469B-88D5-21D761CFE540}">
+  <dimension ref="A1:D68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="393.45" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="100.3" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="162" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="154.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="285.45" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="169.75" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="100.3" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="162" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="378" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="46.3" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="108" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="131.15" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="274.3" x14ac:dyDescent="0.4">
+      <c r="A19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="342.9" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="347.15" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="108" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="239.15" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="254.6" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="192.9" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="154.30000000000001" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="223.75" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="169.75" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>197</v>
+      </c>
+      <c r="B40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" t="s">
+        <v>202</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" t="s">
+        <v>210</v>
+      </c>
+      <c r="C44" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>212</v>
+      </c>
+      <c r="B45" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" t="s">
+        <v>214</v>
+      </c>
+      <c r="D45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>215</v>
+      </c>
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" t="s">
+        <v>217</v>
+      </c>
+      <c r="D46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>218</v>
+      </c>
+      <c r="B47" t="s">
+        <v>219</v>
+      </c>
+      <c r="C47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>221</v>
+      </c>
+      <c r="B48" t="s">
+        <v>222</v>
+      </c>
+      <c r="C48" t="s">
+        <v>223</v>
+      </c>
+      <c r="D48" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" t="s">
+        <v>226</v>
+      </c>
+      <c r="D49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="115.75" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="270" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="177.45" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="401.15" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" t="s">
+        <v>168</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="246.9" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" t="s">
+        <v>180</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="138.9" x14ac:dyDescent="0.4">
+      <c r="A60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="23.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D62" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="216" x14ac:dyDescent="0.4">
+      <c r="A63" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="200.6" x14ac:dyDescent="0.4">
+      <c r="A64" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="123.45" x14ac:dyDescent="0.4">
+      <c r="A65" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="185.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D66" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="239.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="308.60000000000002" x14ac:dyDescent="0.4">
+      <c r="A68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1" xr:uid="{4FFE7EA0-ECB6-471B-878D-58EB5FFE6836}"/>
+    <hyperlink ref="D32" r:id="rId2" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/156863/small.gif" xr:uid="{1DEA380C-4476-4267-882D-2BF7B72CBB84}"/>
+    <hyperlink ref="D31" r:id="rId3" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/152012/small.gif" xr:uid="{F344A039-924F-41CA-A587-30C1EFBECDC0}"/>
+    <hyperlink ref="D30" r:id="rId4" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/169035/small.gif" xr:uid="{3E0FE7AA-35DC-4EAE-923C-546E94CED4B9}"/>
+    <hyperlink ref="D29" r:id="rId5" display="https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/126458/small.gif" xr:uid="{F3AAF613-3FDE-42E0-83F4-4CA8F291BA1C}"/>
+    <hyperlink ref="D67" r:id="rId6" xr:uid="{8CD13B35-BE0A-4B44-A435-05A3065B5EF3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- FINAL TOUCHES ADDED -FIXED FILE PATHS OF ALL FILES
</commit_message>
<xml_diff>
--- a/public/resources/Strategy.xlsx
+++ b/public/resources/Strategy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psn\Desktop\Web Development\Game-hub-server\public\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121915AD-0FB4-437B-B194-24D7C54180CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2462A774-76F3-4A4B-8ED8-F1CA8922B036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" activeTab="7" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="11486" xr2:uid="{AF965BEC-9FC6-4C52-9960-2A6FF7695530}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="280">
   <si>
     <t>NAME</t>
   </si>
@@ -845,6 +845,42 @@
   </si>
   <si>
     <t>"https://img.y8.com/cloud/v2-y8-thumbs-small-thumbnails-001/143474/small.gif"</t>
+  </si>
+  <si>
+    <t>"https://images.crazygames.com/hexa-sort_16x9/20240…at%2Ccompress&amp;q=65&amp;cs=strip&amp;ch=DPR&amp;w=710&amp;fit=crop"</t>
+  </si>
+  <si>
+    <t>Hexa Sort</t>
+  </si>
+  <si>
+    <t>https://www.crazygames.com/game/hexa-sort</t>
+  </si>
+  <si>
+    <t>Hexa Sort is a captivating puzzle game that combines strategic matching and merging challenges. Engage in brain-teasing puzzles where you shuffle and organize hexagon tiles to achieve satisfying color matches. With smooth 3D graphics, vibrant colors, and relaxing gameplay, Hexa Sort offers a perfect balance of excitement and calm, making it ideal for both challenge seekers and those looking to unwind.</t>
+  </si>
+  <si>
+    <t>"https://images.crazygames.com/words-of-wonders_16x…at%2Ccompress&amp;q=65&amp;cs=strip&amp;ch=DPR&amp;w=336&amp;fit=crop"</t>
+  </si>
+  <si>
+    <t>https://www.crazygames.com/game/words-of-wonders</t>
+  </si>
+  <si>
+    <t>Words of Wonder</t>
+  </si>
+  <si>
+    <t>Words of Wonders is a crossword puzzle where you connect letters to reveal hidden words. Test your vocabulary and find all the words to progress and reach more challenging levels. Will you become a master wordsmith in this delightful word game?</t>
+  </si>
+  <si>
+    <t>"https://images.crazygames.com/mergest-kingdom_16x9…at%2Ccompress&amp;q=65&amp;cs=strip&amp;ch=DPR&amp;w=336&amp;fit=crop"</t>
+  </si>
+  <si>
+    <t>https://www.crazygames.com/game/mergest-kingdom</t>
+  </si>
+  <si>
+    <t>Mergest Kingdom</t>
+  </si>
+  <si>
+    <t>Mergest Kingdom is a charming merge puzzle game that lets you build your own kingdom by matching various resources in groups of 3. Start building your fairytale kingdom by completing quests and matching hundreds of objects!</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D1A3C6-19CA-40FA-BFCB-1422A2C32063}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1432,6 +1468,48 @@
       </c>
       <c r="D11" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B12" t="s">
+        <v>270</v>
+      </c>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2446,7 +2524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55908B1F-4066-469B-88D5-21D761CFE540}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>